<commit_message>
evaluated and compared the variants of CRO
</commit_message>
<xml_diff>
--- a/CRO_SL_python.xlsx
+++ b/CRO_SL_python.xlsx
@@ -98,7 +98,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00E+00"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,16 +117,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAAAAAA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -146,20 +163,113 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.00E+00"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9DC3E6"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.00E+00"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.00E+00"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -449,7 +559,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -978,19 +1088,72 @@
         <v>2.145796145320206E-09</v>
       </c>
     </row>
+    <row r="18" spans="1:10">
+      <c r="B18" s="2">
+        <f t="array" ref="B18">(AVERAGE(B3:B17))</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="array" ref="C18">(AVERAGE(C3:C17))</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="array" ref="D18">(AVERAGE(D3:D17))</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="array" ref="E18">(AVERAGE(E3:E17))</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="array" ref="F18">(AVERAGE(F3:F17))</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="array" ref="G18">(AVERAGE(G3:G17))</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="array" ref="H18">(AVERAGE(H3:H17))</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="array" ref="I18">(AVERAGE(I3:I17))</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="array" ref="J18">(AVERAGE(J3:J17))</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:D17">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:G17">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:J17">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1519,19 +1682,72 @@
         <v>1.138371985030072E-08</v>
       </c>
     </row>
+    <row r="18" spans="1:10">
+      <c r="B18" s="2">
+        <f t="array" ref="B18">(AVERAGE(B3:B17))</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="array" ref="C18">(AVERAGE(C3:C17))</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="array" ref="D18">(AVERAGE(D3:D17))</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="array" ref="E18">(AVERAGE(E3:E17))</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="array" ref="F18">(AVERAGE(F3:F17))</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="array" ref="G18">(AVERAGE(G3:G17))</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="array" ref="H18">(AVERAGE(H3:H17))</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="array" ref="I18">(AVERAGE(I3:I17))</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="array" ref="J18">(AVERAGE(J3:J17))</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:D17">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:G17">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:J17">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2060,19 +2276,72 @@
         <v>0.0172142839237705</v>
       </c>
     </row>
+    <row r="18" spans="1:10">
+      <c r="B18" s="2">
+        <f t="array" ref="B18">(AVERAGE(B3:B17))</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="array" ref="C18">(AVERAGE(C3:C17))</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="array" ref="D18">(AVERAGE(D3:D17))</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="array" ref="E18">(AVERAGE(E3:E17))</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="array" ref="F18">(AVERAGE(F3:F17))</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="array" ref="G18">(AVERAGE(G3:G17))</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="array" ref="H18">(AVERAGE(H3:H17))</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="array" ref="I18">(AVERAGE(I3:I17))</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="array" ref="J18">(AVERAGE(J3:J17))</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:D17">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:G17">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:J17">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2601,19 +2870,72 @@
         <v>1.773889114557588</v>
       </c>
     </row>
+    <row r="18" spans="1:10">
+      <c r="B18" s="2">
+        <f t="array" ref="B18">(AVERAGE(B3:B17))</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="array" ref="C18">(AVERAGE(C3:C17))</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="array" ref="D18">(AVERAGE(D3:D17))</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="array" ref="E18">(AVERAGE(E3:E17))</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="array" ref="F18">(AVERAGE(F3:F17))</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="array" ref="G18">(AVERAGE(G3:G17))</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="array" ref="H18">(AVERAGE(H3:H17))</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="array" ref="I18">(AVERAGE(I3:I17))</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="array" ref="J18">(AVERAGE(J3:J17))</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:D17">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:G17">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:J17">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3142,19 +3464,72 @@
         <v>0.013119198883474</v>
       </c>
     </row>
+    <row r="18" spans="1:10">
+      <c r="B18" s="2">
+        <f t="array" ref="B18">(AVERAGE(B3:B17))</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="array" ref="C18">(AVERAGE(C3:C17))</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="array" ref="D18">(AVERAGE(D3:D17))</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="array" ref="E18">(AVERAGE(E3:E17))</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="array" ref="F18">(AVERAGE(F3:F17))</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="array" ref="G18">(AVERAGE(G3:G17))</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="array" ref="H18">(AVERAGE(H3:H17))</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="array" ref="I18">(AVERAGE(I3:I17))</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="array" ref="J18">(AVERAGE(J3:J17))</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:D17">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:G17">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:J17">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3683,19 +4058,72 @@
         <v>0.0031276132641161</v>
       </c>
     </row>
+    <row r="18" spans="1:10">
+      <c r="B18" s="2">
+        <f t="array" ref="B18">(AVERAGE(B3:B17))</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="array" ref="C18">(AVERAGE(C3:C17))</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="array" ref="D18">(AVERAGE(D3:D17))</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="array" ref="E18">(AVERAGE(E3:E17))</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="array" ref="F18">(AVERAGE(F3:F17))</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="array" ref="G18">(AVERAGE(G3:G17))</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="array" ref="H18">(AVERAGE(H3:H17))</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="array" ref="I18">(AVERAGE(I3:I17))</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="array" ref="J18">(AVERAGE(J3:J17))</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:D17">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:G17">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:J17">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4224,19 +4652,72 @@
         <v>1.245028690637071E-11</v>
       </c>
     </row>
+    <row r="18" spans="1:10">
+      <c r="B18" s="2">
+        <f t="array" ref="B18">(AVERAGE(B3:B17))</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="array" ref="C18">(AVERAGE(C3:C17))</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="array" ref="D18">(AVERAGE(D3:D17))</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="array" ref="E18">(AVERAGE(E3:E17))</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="array" ref="F18">(AVERAGE(F3:F17))</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="array" ref="G18">(AVERAGE(G3:G17))</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="array" ref="H18">(AVERAGE(H3:H17))</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="array" ref="I18">(AVERAGE(I3:I17))</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="array" ref="J18">(AVERAGE(J3:J17))</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:D17">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:G17">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:J17">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4765,19 +5246,72 @@
         <v>0.8259358496315955</v>
       </c>
     </row>
+    <row r="18" spans="1:10">
+      <c r="B18" s="2">
+        <f t="array" ref="B18">(AVERAGE(B3:B17))</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="array" ref="C18">(AVERAGE(C3:C17))</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="array" ref="D18">(AVERAGE(D3:D17))</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="array" ref="E18">(AVERAGE(E3:E17))</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="array" ref="F18">(AVERAGE(F3:F17))</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="array" ref="G18">(AVERAGE(G3:G17))</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="array" ref="H18">(AVERAGE(H3:H17))</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="array" ref="I18">(AVERAGE(I3:I17))</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="array" ref="J18">(AVERAGE(J3:J17))</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:D17">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:G17">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:J17">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5306,19 +5840,72 @@
         <v>1.104848865296326E-06</v>
       </c>
     </row>
+    <row r="18" spans="1:10">
+      <c r="B18" s="2">
+        <f t="array" ref="B18">(AVERAGE(B3:B17))</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="array" ref="C18">(AVERAGE(C3:C17))</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="array" ref="D18">(AVERAGE(D3:D17))</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="array" ref="E18">(AVERAGE(E3:E17))</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="array" ref="F18">(AVERAGE(F3:F17))</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="array" ref="G18">(AVERAGE(G3:G17))</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="array" ref="H18">(AVERAGE(H3:H17))</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="array" ref="I18">(AVERAGE(I3:I17))</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="array" ref="J18">(AVERAGE(J3:J17))</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:D17">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:G17">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:J17">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5847,19 +6434,72 @@
         <v>6.943715037867571E-14</v>
       </c>
     </row>
+    <row r="18" spans="1:10">
+      <c r="B18" s="2">
+        <f t="array" ref="B18">(AVERAGE(B3:B17))</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="array" ref="C18">(AVERAGE(C3:C17))</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="array" ref="D18">(AVERAGE(D3:D17))</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="array" ref="E18">(AVERAGE(E3:E17))</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="array" ref="F18">(AVERAGE(F3:F17))</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="array" ref="G18">(AVERAGE(G3:G17))</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="array" ref="H18">(AVERAGE(H3:H17))</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="array" ref="I18">(AVERAGE(I3:I17))</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="array" ref="J18">(AVERAGE(J3:J17))</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:D17">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:G17">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:J17">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6388,19 +7028,72 @@
         <v>2.39682207533547E-10</v>
       </c>
     </row>
+    <row r="18" spans="1:10">
+      <c r="B18" s="2">
+        <f t="array" ref="B18">(AVERAGE(B3:B17))</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="array" ref="C18">(AVERAGE(C3:C17))</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="array" ref="D18">(AVERAGE(D3:D17))</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="array" ref="E18">(AVERAGE(E3:E17))</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="array" ref="F18">(AVERAGE(F3:F17))</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="array" ref="G18">(AVERAGE(G3:G17))</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="array" ref="H18">(AVERAGE(H3:H17))</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="array" ref="I18">(AVERAGE(I3:I17))</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="array" ref="J18">(AVERAGE(J3:J17))</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:D17">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:G17">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:J17">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6929,19 +7622,72 @@
         <v>7.901827198543009</v>
       </c>
     </row>
+    <row r="18" spans="1:10">
+      <c r="B18" s="2">
+        <f t="array" ref="B18">(AVERAGE(B3:B17))</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="array" ref="C18">(AVERAGE(C3:C17))</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="array" ref="D18">(AVERAGE(D3:D17))</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="array" ref="E18">(AVERAGE(E3:E17))</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="array" ref="F18">(AVERAGE(F3:F17))</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="array" ref="G18">(AVERAGE(G3:G17))</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="array" ref="H18">(AVERAGE(H3:H17))</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="array" ref="I18">(AVERAGE(I3:I17))</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="array" ref="J18">(AVERAGE(J3:J17))</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:D17">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:G17">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:J17">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7470,12 +8216,65 @@
         <v>6.029954262470932E-10</v>
       </c>
     </row>
+    <row r="18" spans="1:10">
+      <c r="B18" s="2">
+        <f t="array" ref="B18">(AVERAGE(B3:B17))</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="array" ref="C18">(AVERAGE(C3:C17))</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="array" ref="D18">(AVERAGE(D3:D17))</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="array" ref="E18">(AVERAGE(E3:E17))</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="array" ref="F18">(AVERAGE(F3:F17))</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="array" ref="G18">(AVERAGE(G3:G17))</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="array" ref="H18">(AVERAGE(H3:H17))</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="array" ref="I18">(AVERAGE(I3:I17))</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="array" ref="J18">(AVERAGE(J3:J17))</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:D17">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:G17">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:J17">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+      <formula>Dummy</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>